<commit_message>
Actializacion de repocitorio: Finalizacion
</commit_message>
<xml_diff>
--- a/src/test/resources/data/dataExcel.xlsx
+++ b/src/test/resources/data/dataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roana\IdeaProjects\Trabajo_POM_ronald_veas\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B51087B-6263-4235-95D2-8286C4B2F904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E74919-B5C0-45D3-9C71-9AFC94AA7D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{90BA81F5-CB8F-49BA-8F1A-F47E825CE830}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Dato1</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t>Enero</t>
+  </si>
+  <si>
+    <t>https://www.pcfactory.cl/misdatos</t>
+  </si>
+  <si>
+    <t>https://www.condorito.com/</t>
+  </si>
+  <si>
+    <t>RUT o Numero de boleta incorrecto</t>
   </si>
 </sst>
 </file>
@@ -611,15 +620,15 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="8" max="8" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -698,7 +707,9 @@
       <c r="C3" s="4">
         <v>8768928433</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -719,7 +730,9 @@
       <c r="C4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -737,8 +750,10 @@
       <c r="B5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>

</xml_diff>